<commit_message>
basic establish research ms
</commit_message>
<xml_diff>
--- a/src/main/java/com/buct/graduation/util/excel/综合评价结果模板.xlsx
+++ b/src/main/java/com/buct/graduation/util/excel/综合评价结果模板.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20357"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20358"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\reporter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\JavaWeb\毕业设计\graduation\src\main\java\com\buct\graduation\util\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D883F102-55F7-4B90-8F36-19F87F70C2DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD40F4C-9CE5-4302-AB19-3B32A21DF0A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22935" yWindow="-15" windowWidth="23250" windowHeight="12570" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22935" yWindow="-15" windowWidth="23250" windowHeight="12570" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="基本信息" sheetId="2" r:id="rId1"/>
@@ -374,15 +374,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>${item.journal.isTop}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>${item.journal.IF}</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>${item.isESI}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -679,6 +671,14 @@
       </rPr>
       <t>}</t>
     </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${item.journal.is_top}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${item.is_esi}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1110,6 +1110,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1124,38 +1127,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1163,6 +1134,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1170,10 +1144,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1470,11 +1470,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
@@ -1488,7 +1488,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="30" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="17" t="s">
@@ -1499,7 +1499,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
+      <c r="A4" s="31"/>
       <c r="B4" s="19" t="s">
         <v>50</v>
       </c>
@@ -1555,11 +1555,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
@@ -1574,12 +1574,12 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
         <v>86</v>
@@ -1621,11 +1621,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
@@ -1640,12 +1640,12 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
         <v>86</v>
@@ -1675,8 +1675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D69549-01EA-49D7-A578-ACA7554E41E5}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1692,17 +1692,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
@@ -1735,12 +1735,12 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
         <v>86</v>
@@ -1752,16 +1752,16 @@
         <v>93</v>
       </c>
       <c r="E4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F4" t="s">
         <v>97</v>
-      </c>
-      <c r="F4" t="s">
-        <v>98</v>
       </c>
       <c r="G4" t="s">
         <v>96</v>
       </c>
       <c r="H4" t="s">
-        <v>99</v>
+        <v>137</v>
       </c>
       <c r="I4" t="s">
         <v>89</v>
@@ -1800,14 +1800,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
@@ -1831,12 +1831,12 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
         <v>86</v>
@@ -1872,7 +1872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
@@ -1901,10 +1901,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="B1" s="37"/>
+      <c r="A1" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="55"/>
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
       <c r="E1" s="38"/>
@@ -1928,29 +1928,29 @@
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="33"/>
+        <v>107</v>
+      </c>
+      <c r="C2" s="52"/>
       <c r="D2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="42"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="47"/>
     </row>
     <row r="3" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
@@ -1959,39 +1959,39 @@
       <c r="B3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C3" s="34"/>
+      <c r="C3" s="53"/>
       <c r="D3" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G3" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="L3" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="47"/>
+      <c r="N3" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="L3" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" s="42"/>
-      <c r="N3" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="O3" s="43" t="s">
+      <c r="O3" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="42"/>
+      <c r="P3" s="47"/>
       <c r="Q3" s="5"/>
-      <c r="R3" s="44"/>
-      <c r="S3" s="42"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="47"/>
     </row>
     <row r="4" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
@@ -2000,178 +2000,178 @@
       <c r="B4" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="34"/>
+      <c r="C4" s="53"/>
       <c r="D4" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="47"/>
+      <c r="K4" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="L4" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="47"/>
+      <c r="N4" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="G4" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="41"/>
-      <c r="I4" s="41"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="L4" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" s="42"/>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="O4" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="R4" s="43" t="s">
+      <c r="R4" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="S4" s="42"/>
+      <c r="S4" s="47"/>
     </row>
     <row r="5" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="C5" s="34"/>
+        <v>104</v>
+      </c>
+      <c r="C5" s="53"/>
       <c r="D5" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="47"/>
+      <c r="K5" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="G5" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="M5" s="47"/>
+      <c r="N5" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="O5" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="L5" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="M5" s="42"/>
-      <c r="N5" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="O5" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="R5" s="43" t="s">
+      <c r="R5" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="S5" s="42"/>
+      <c r="S5" s="47"/>
     </row>
     <row r="6" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C6" s="34"/>
+        <v>105</v>
+      </c>
+      <c r="C6" s="53"/>
       <c r="D6" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="L6" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="47"/>
+      <c r="N6" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="G6" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="5" t="s">
+      <c r="O6" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="L6" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" s="42"/>
-      <c r="N6" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="O6" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="R6" s="43" t="s">
+      <c r="R6" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="42"/>
+      <c r="S6" s="47"/>
     </row>
     <row r="7" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="55" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" s="56" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="53"/>
+      <c r="D7" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="45" t="s">
         <v>27</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="L7" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="47"/>
+      <c r="N7" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="G7" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="5" t="s">
+      <c r="O7" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" s="47"/>
+      <c r="Q7" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="L7" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" s="42"/>
-      <c r="N7" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="O7" s="43" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="R7" s="43" t="s">
+      <c r="R7" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="S7" s="42"/>
+      <c r="S7" s="47"/>
     </row>
     <row r="8" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -2180,35 +2180,35 @@
       <c r="B8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>32</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="I8" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="I8" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="42"/>
-      <c r="K8" s="57" t="s">
-        <v>137</v>
-      </c>
-      <c r="L8" s="43" t="s">
+      <c r="J8" s="47"/>
+      <c r="K8" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="L8" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="M8" s="41"/>
-      <c r="N8" s="41"/>
-      <c r="O8" s="41"/>
-      <c r="P8" s="42"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="47"/>
       <c r="Q8" s="10"/>
-      <c r="R8" s="44"/>
-      <c r="S8" s="42"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="47"/>
     </row>
     <row r="9" spans="1:19" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
@@ -2217,45 +2217,45 @@
       <c r="B9" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C9" s="34"/>
+      <c r="C9" s="53"/>
       <c r="D9" s="7" t="s">
         <v>36</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="48"/>
-      <c r="S9" s="49"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="35"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="35"/>
+      <c r="O9" s="35"/>
+      <c r="P9" s="35"/>
+      <c r="Q9" s="35"/>
+      <c r="R9" s="35"/>
+      <c r="S9" s="36"/>
     </row>
     <row r="10" spans="1:19" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C10" s="34"/>
+        <v>98</v>
+      </c>
+      <c r="C10" s="53"/>
       <c r="D10" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="50"/>
+      <c r="F10" s="37"/>
       <c r="G10" s="38"/>
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
@@ -2268,23 +2268,23 @@
       <c r="P10" s="38"/>
       <c r="Q10" s="38"/>
       <c r="R10" s="38"/>
-      <c r="S10" s="51"/>
+      <c r="S10" s="39"/>
     </row>
     <row r="11" spans="1:19" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="34"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="9" t="s">
         <v>42</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="50"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="38"/>
       <c r="H11" s="38"/>
       <c r="I11" s="38"/>
@@ -2297,51 +2297,36 @@
       <c r="P11" s="38"/>
       <c r="Q11" s="38"/>
       <c r="R11" s="38"/>
-      <c r="S11" s="51"/>
+      <c r="S11" s="39"/>
     </row>
     <row r="12" spans="1:19" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="9" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="52"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="53"/>
-      <c r="Q12" s="53"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="54"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="42"/>
     </row>
     <row r="16" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="F9:S12"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="R8:S8"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="L8:P8"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="G7:J7"/>
     <mergeCell ref="C2:C12"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A11:A12"/>
@@ -2358,6 +2343,21 @@
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="R3:S3"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="L8:P8"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="F9:S12"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="I8:J8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>